<commit_message>
Pequeños cambios de funcionalidad a los formularios
</commit_message>
<xml_diff>
--- a/Modelo datos.xlsx
+++ b/Modelo datos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAA6FAAC-7C9F-4DA7-9BCB-FAC3FFF759B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B8FD74-7481-4C99-A2EE-037B6CD038C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1065" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>Materiales</t>
   </si>
@@ -143,9 +143,6 @@
     <t>fecha_mant</t>
   </si>
   <si>
-    <t>id_empleado</t>
-  </si>
-  <si>
     <t>RespXMatenimi</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>Patente</t>
   </si>
   <si>
-    <t>Stock_Repuestos</t>
-  </si>
-  <si>
     <t>nro_doc_responsable</t>
   </si>
   <si>
@@ -273,6 +267,12 @@
   </si>
   <si>
     <t>cuit_cliente</t>
+  </si>
+  <si>
+    <t>legajo_empleado</t>
+  </si>
+  <si>
+    <t>RepuestosXProov</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +380,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -472,11 +478,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,41 +592,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,14 +1093,14 @@
         <v>13</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" s="16"/>
       <c r="M3" s="28" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="16"/>
@@ -1097,10 +1127,10 @@
       <c r="H4" s="16"/>
       <c r="I4" s="45"/>
       <c r="J4" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="11"/>
@@ -1136,7 +1166,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="16"/>
@@ -1155,10 +1185,10 @@
       <c r="D6" s="14"/>
       <c r="E6" s="3"/>
       <c r="F6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="11"/>
@@ -1169,7 +1199,7 @@
       <c r="L6" s="16"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="16"/>
@@ -1178,7 +1208,7 @@
         <v>25</v>
       </c>
       <c r="S6" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T6" s="15"/>
       <c r="U6" s="1"/>
@@ -1190,18 +1220,18 @@
       <c r="D7" s="14"/>
       <c r="E7" s="3"/>
       <c r="F7" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="11"/>
       <c r="J7" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="16"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="16"/>
@@ -1348,7 +1378,7 @@
       <c r="P13" s="15"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="15"/>
@@ -1356,14 +1386,14 @@
     </row>
     <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="14"/>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="39" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="20" t="s">
@@ -1374,32 +1404,36 @@
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="15"/>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="39" t="s">
         <v>11</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="P14" s="15"/>
-      <c r="Q14" s="41" t="s">
+      <c r="Q14" s="39" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S14" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="S14" s="47" t="s">
+        <v>59</v>
+      </c>
       <c r="T14" s="15"/>
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="14"/>
-      <c r="E15" s="42"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="1"/>
@@ -1408,17 +1442,21 @@
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="43"/>
+      <c r="M15" s="40"/>
       <c r="N15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O15" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="P15" s="15"/>
-      <c r="Q15" s="43"/>
+      <c r="Q15" s="40"/>
       <c r="R15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S15" s="1"/>
+      <c r="S15" s="39" t="s">
+        <v>59</v>
+      </c>
       <c r="T15" s="15"/>
       <c r="U15" s="1"/>
     </row>
@@ -1435,17 +1473,17 @@
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="42"/>
+      <c r="M16" s="41"/>
       <c r="N16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="15"/>
-      <c r="Q16" s="43"/>
-      <c r="R16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S16" s="1"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="S16" s="40"/>
       <c r="T16" s="15"/>
       <c r="U16" s="1"/>
     </row>
@@ -1464,11 +1502,11 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="15"/>
-      <c r="Q17" s="42"/>
+      <c r="Q17" s="41"/>
       <c r="R17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S17" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="S17" s="41"/>
       <c r="T17" s="15"/>
       <c r="U17" s="1"/>
     </row>
@@ -1484,12 +1522,11 @@
       <c r="K18" s="1"/>
       <c r="L18" s="15"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="15"/>
@@ -1507,11 +1544,9 @@
       <c r="K19" s="1"/>
       <c r="L19" s="15"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="15"/>
       <c r="U19" s="1"/>
@@ -1597,13 +1632,13 @@
       <c r="H25" s="15"/>
       <c r="I25" s="1"/>
       <c r="J25" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="15"/>
       <c r="M25" s="1"/>
       <c r="N25" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="15"/>
@@ -1689,7 +1724,7 @@
       <c r="L28" s="15"/>
       <c r="M28" s="1"/>
       <c r="N28" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="15"/>
@@ -1716,7 +1751,7 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="15"/>
@@ -1740,7 +1775,7 @@
       <c r="L31" s="14"/>
       <c r="P31" s="14"/>
       <c r="R31" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="15"/>
@@ -1784,7 +1819,7 @@
       <c r="P33" s="14"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S33" s="3"/>
       <c r="T33" s="14"/>
@@ -1873,21 +1908,21 @@
     </row>
     <row r="40" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="14"/>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="39" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="41" t="s">
+      <c r="I40" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>28</v>
+      <c r="J40" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="15"/>
@@ -1903,7 +1938,7 @@
         <v>11</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S40" s="1"/>
       <c r="T40" s="15"/>
@@ -1911,17 +1946,17 @@
     </row>
     <row r="41" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D41" s="14"/>
-      <c r="E41" s="42"/>
+      <c r="E41" s="41"/>
       <c r="F41" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H41" s="15"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="17" t="s">
-        <v>32</v>
+      <c r="I41" s="48"/>
+      <c r="J41" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="15"/>
@@ -1936,7 +1971,7 @@
         <v>25</v>
       </c>
       <c r="S41" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T41" s="15"/>
       <c r="U41" s="1"/>
@@ -1948,23 +1983,23 @@
       <c r="H42" s="15"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O42" s="20" t="s">
         <v>59</v>
-      </c>
-      <c r="O42" s="20" t="s">
-        <v>60</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S42" s="1"/>
       <c r="T42" s="15"/>
@@ -1979,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="K43" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="1"/>
@@ -1988,7 +2023,7 @@
       <c r="P43" s="15"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S43" s="1"/>
       <c r="T43" s="15"/>
@@ -2014,8 +2049,8 @@
     <row r="45" spans="4:21" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="40"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="38"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
@@ -2115,37 +2150,37 @@
       <c r="H51" s="15"/>
       <c r="I51" s="1"/>
       <c r="J51" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="1"/>
       <c r="N51" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P51" s="15"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="21" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="T51" s="14"/>
     </row>
     <row r="52" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="14"/>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="39" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H52" s="15"/>
-      <c r="I52" s="41" t="s">
+      <c r="I52" s="39" t="s">
         <v>11</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K52" s="1"/>
       <c r="L52" s="15"/>
@@ -2153,34 +2188,34 @@
         <v>11</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="15"/>
-      <c r="Q52" s="20" t="s">
+      <c r="Q52" s="39" t="s">
         <v>11</v>
       </c>
       <c r="R52" s="11" t="s">
         <v>23</v>
       </c>
       <c r="S52" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T52" s="15"/>
     </row>
     <row r="53" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="14"/>
-      <c r="E53" s="42"/>
+      <c r="E53" s="41"/>
       <c r="F53" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H53" s="15"/>
-      <c r="I53" s="42"/>
+      <c r="I53" s="41"/>
       <c r="J53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K53" s="1"/>
       <c r="L53" s="15"/>
@@ -2190,19 +2225,19 @@
       </c>
       <c r="O53" s="1"/>
       <c r="P53" s="15"/>
-      <c r="Q53" s="1"/>
+      <c r="Q53" s="41"/>
       <c r="R53" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S53" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T53" s="15"/>
     </row>
     <row r="54" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D54" s="14"/>
       <c r="F54" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="15"/>
@@ -2221,13 +2256,13 @@
     <row r="55" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="14"/>
       <c r="F55" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="15"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L55" s="15"/>
       <c r="M55" s="1"/>
@@ -2240,7 +2275,7 @@
     <row r="56" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="14"/>
       <c r="F56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="15"/>
@@ -2249,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="K56" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="1"/>
@@ -2262,7 +2297,7 @@
     <row r="57" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D57" s="14"/>
       <c r="F57" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H57" s="14"/>
       <c r="L57" s="14"/>
@@ -2355,25 +2390,25 @@
     <row r="63" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="14"/>
       <c r="F63" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="15"/>
       <c r="I63" s="4"/>
       <c r="J63" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="15"/>
       <c r="M63" s="4"/>
       <c r="N63" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O63" s="4"/>
       <c r="P63" s="15"/>
       <c r="Q63" s="4"/>
       <c r="R63" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S63" s="4"/>
       <c r="T63" s="15"/>
@@ -2384,7 +2419,7 @@
         <v>11</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G64" s="9"/>
       <c r="H64" s="16"/>
@@ -2392,7 +2427,7 @@
         <v>11</v>
       </c>
       <c r="J64" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K64" s="23"/>
       <c r="L64" s="16"/>
@@ -2400,18 +2435,18 @@
         <v>11</v>
       </c>
       <c r="N64" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O64" s="23"/>
       <c r="P64" s="16"/>
-      <c r="Q64" s="37" t="s">
+      <c r="Q64" s="44" t="s">
         <v>11</v>
       </c>
       <c r="R64" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S64" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T64" s="16"/>
     </row>
@@ -2424,11 +2459,8 @@
       <c r="G65" s="10"/>
       <c r="H65" s="16"/>
       <c r="I65" s="24"/>
-      <c r="J65" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="K65" s="28" t="s">
-        <v>60</v>
+      <c r="J65" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="L65" s="16"/>
       <c r="M65" s="11"/>
@@ -2437,12 +2469,12 @@
       </c>
       <c r="O65" s="23"/>
       <c r="P65" s="16"/>
-      <c r="Q65" s="38"/>
+      <c r="Q65" s="46"/>
       <c r="R65" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S65" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T65" s="16"/>
     </row>
@@ -2454,46 +2486,45 @@
       <c r="H66" s="16"/>
       <c r="I66" s="24"/>
       <c r="J66" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K66" s="28" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="L66" s="16"/>
       <c r="M66" s="11"/>
       <c r="N66" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O66" s="9"/>
       <c r="P66" s="16"/>
       <c r="Q66" s="24"/>
       <c r="R66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S66" s="9"/>
       <c r="T66" s="16"/>
     </row>
-    <row r="67" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D67" s="14"/>
       <c r="E67" s="3"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="16"/>
       <c r="I67" s="9"/>
-      <c r="J67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K67" s="9"/>
+      <c r="J67" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K67" s="28" t="s">
+        <v>59</v>
+      </c>
       <c r="L67" s="16"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O67" s="9"/>
       <c r="P67" s="16"/>
       <c r="Q67" s="9"/>
       <c r="R67" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S67" s="9"/>
       <c r="T67" s="16"/>
@@ -2506,13 +2537,15 @@
       <c r="H68" s="16"/>
       <c r="I68" s="11"/>
       <c r="J68" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K68" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="K68" s="28" t="s">
+        <v>59</v>
+      </c>
       <c r="L68" s="16"/>
       <c r="M68" s="11"/>
       <c r="N68" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68" s="16"/>
@@ -2520,19 +2553,14 @@
       <c r="S68" s="11"/>
       <c r="T68" s="16"/>
     </row>
-    <row r="69" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D69" s="14"/>
       <c r="E69" s="3"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="16"/>
       <c r="I69" s="11"/>
-      <c r="J69" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K69" s="28" t="s">
-        <v>60</v>
-      </c>
+      <c r="K69" s="50"/>
       <c r="L69" s="16"/>
       <c r="M69" s="11"/>
       <c r="O69" s="11"/>
@@ -2582,38 +2610,38 @@
       <c r="D75" s="14"/>
       <c r="E75" s="3"/>
       <c r="F75" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="15"/>
     </row>
     <row r="76" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D76" s="14"/>
-      <c r="E76" s="41" t="s">
+      <c r="E76" s="39" t="s">
         <v>11</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G76" s="47" t="s">
-        <v>60</v>
+        <v>80</v>
+      </c>
+      <c r="G76" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="H76" s="16"/>
     </row>
     <row r="77" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="14"/>
-      <c r="E77" s="43"/>
+      <c r="E77" s="40"/>
       <c r="F77" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G77" s="48"/>
+        <v>79</v>
+      </c>
+      <c r="G77" s="43"/>
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="14"/>
-      <c r="E78" s="42"/>
+      <c r="E78" s="41"/>
       <c r="F78" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G78" s="9"/>
       <c r="H78" s="16"/>
@@ -2654,17 +2682,19 @@
       <c r="H83" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="Q64:Q65"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="M14:M16"/>
     <mergeCell ref="E76:E78"/>
     <mergeCell ref="G76:G77"/>
     <mergeCell ref="E52:E53"/>
     <mergeCell ref="I52:I53"/>
     <mergeCell ref="Q14:Q17"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="I40:I41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>